<commit_message>
enhanced the vesselconnectivity logic
</commit_message>
<xml_diff>
--- a/src/test/resources/EnvironmentData.xlsx
+++ b/src/test/resources/EnvironmentData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t xml:space="preserve">Environment</t>
   </si>
@@ -34,19 +34,61 @@
     <t xml:space="preserve">PROD</t>
   </si>
   <si>
+    <t xml:space="preserve">imc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">chellship</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imc</t>
-  </si>
-  <si>
     <t xml:space="preserve">orion</t>
   </si>
   <si>
+    <t xml:space="preserve">asiaticlloyd</t>
+  </si>
+  <si>
     <t xml:space="preserve">kitaura-kaiun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aesm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gesco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abo-shoten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mlepchems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v-ships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prime-tankers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imecs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sevenislands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">misuga-kaiun</t>
   </si>
   <si>
     <t xml:space="preserve">UAT</t>
@@ -143,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -152,19 +194,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -361,10 +395,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,115 +406,262 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="2" width="9.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="9.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="6"/>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C20" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Implemented headless execution support
</commit_message>
<xml_diff>
--- a/src/test/resources/EnvironmentData.xlsx
+++ b/src/test/resources/EnvironmentData.xlsx
@@ -46,10 +46,10 @@
     <t xml:space="preserve">orion</t>
   </si>
   <si>
+    <t xml:space="preserve">asiaticlloyd</t>
+  </si>
+  <si>
     <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asiaticlloyd</t>
   </si>
   <si>
     <t xml:space="preserve">kitaura-kaiun</t>
@@ -398,7 +398,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,7 +455,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -466,10 +466,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -516,7 +516,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>